<commit_message>
Add main_manager field to target_program
</commit_message>
<xml_diff>
--- a/public/files/target_programs/import/import_template.xlsx
+++ b/public/files/target_programs/import/import_template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
   <si>
     <t>MANAGER</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>MAIN_MANAGER</t>
   </si>
   <si>
     <t>Київська міська рада (Секретаріат)</t>
@@ -79,6 +82,9 @@
   </si>
   <si>
     <t>3 652.3</t>
+  </si>
+  <si>
+    <t>Апарат виконавчого органу Київської міської ради (КМДА)</t>
   </si>
   <si>
     <t>Бюджетний кодекс України</t>
@@ -346,7 +352,7 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -398,10 +404,13 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>110170</v>
@@ -413,28 +422,31 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>61658.4</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>2016</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -446,19 +458,19 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I42" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M42" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N42" s="0" t="n">
         <v>2</v>
       </c>
       <c r="O42" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P42" s="0" t="n">
         <v>3400</v>
@@ -466,40 +478,40 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I43" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I44" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I45" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I46" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I47" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I48" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I49" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +551,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>8</v>
@@ -553,7 +565,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>3</v>
@@ -567,7 +579,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
@@ -581,7 +593,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
@@ -626,33 +638,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>175</v>
@@ -660,16 +672,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>112300</v>
@@ -677,16 +689,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3400</v>
@@ -694,16 +706,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>641.7</v>
@@ -711,16 +723,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>19.4</v>
@@ -728,16 +740,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>302.7</v>
@@ -745,16 +757,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>7342</v>
@@ -762,16 +774,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3892</v>
@@ -779,16 +791,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>212</v>
@@ -796,16 +808,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>3238</v>
@@ -813,30 +825,30 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>19723.7</v>
@@ -844,16 +856,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>18244</v>
@@ -861,10 +873,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2</v>
@@ -872,16 +884,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>2.47</v>
@@ -889,16 +901,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>24.288</v>
@@ -906,16 +918,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1666.79</v>
@@ -923,10 +935,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>3</v>
@@ -934,16 +946,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>0.14</v>
@@ -951,16 +963,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1.231</v>
@@ -968,16 +980,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>84.5</v>
@@ -985,10 +997,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>4</v>
@@ -996,72 +1008,72 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>100</v>
@@ -1069,16 +1081,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3549.1</v>
@@ -1086,16 +1098,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>206</v>
@@ -1103,16 +1115,16 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>3</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>17.2</v>
@@ -1120,16 +1132,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>100</v>

</xml_diff>